<commit_message>
Updates to pessoas and codes
</commit_message>
<xml_diff>
--- a/Hluvukani_C1_prova_vida/Hluvukani_C1_prova_vida-media/Hluvukani_C1_prova_vida.xlsx
+++ b/Hluvukani_C1_prova_vida/Hluvukani_C1_prova_vida-media/Hluvukani_C1_prova_vida.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18827"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7380" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="175">
   <si>
     <t>type</t>
   </si>
@@ -285,130 +285,274 @@
 Por favor deslizar para a frente para continuar.</t>
   </si>
   <si>
-    <t>Chiconela Ezequiel fenias c_impost 5610</t>
-  </si>
-  <si>
-    <t>Chiconela Isaque Fenias Chiconela c_impost 5610</t>
-  </si>
-  <si>
-    <t>Chicuamba Ismael Alfredo bi 100404696751Q</t>
-  </si>
-  <si>
-    <t>Chilaule Maria Azarias bi 1004026800497N</t>
-  </si>
-  <si>
-    <t>Chilaule Maria Azarias ced 668046</t>
-  </si>
-  <si>
-    <t>Chivure Celeste Gabriel Novela bi 110201649569Q</t>
-  </si>
-  <si>
-    <t>Dolhana Maria João bi 100404559519P</t>
-  </si>
-  <si>
-    <t>Hunguana Sérgio Gonçalves bi 110101036908C</t>
-  </si>
-  <si>
-    <t>Komaio Albertina Kei c_eleit 12071563</t>
-  </si>
-  <si>
-    <t>Livisse Agostinho João bi 110104642611N</t>
-  </si>
-  <si>
-    <t>Lumbela Elias Machelagodine bi 110100295545A</t>
-  </si>
-  <si>
-    <t>Macamo Angelo Luis c_eleit 12071794</t>
-  </si>
-  <si>
-    <t>Machaeie Benedito Diniz ced 65146</t>
-  </si>
-  <si>
-    <t>Machaeie José Diniz ced 857421</t>
-  </si>
-  <si>
-    <t>Machaieie Benedito Dinis ced 65146</t>
-  </si>
-  <si>
-    <t>Machaieie Maria Azarias Chilaule bi 100402680497N</t>
-  </si>
-  <si>
-    <t>Machiana Carla Isabel p_port 15AJ41963</t>
-  </si>
-  <si>
-    <t>Macuacua Flora Silvestre c_eleit 1004A860810839</t>
-  </si>
-  <si>
-    <t>Macuacua Marta Causolada c_eleit 13082829</t>
-  </si>
-  <si>
-    <t>MANHIÇA Isabel Joaquim bi 10006696B</t>
-  </si>
-  <si>
-    <t>MANHIÇA LAURINDA JOAQUIM c_eleit 367707</t>
-  </si>
-  <si>
-    <t>MANHIÇA Violeta Cotassana bi 100400613064B</t>
-  </si>
-  <si>
-    <t>Mapanga Lúcia Clarmina bi 100400667510Q</t>
-  </si>
-  <si>
-    <t>Massango Mónica Amone bi 110101302568F</t>
-  </si>
-  <si>
-    <t>Mawelele Leonardo Fabião c_eleit 12598423</t>
-  </si>
-  <si>
-    <t>Mbeve Ana Maria Antónia bi 100005272F</t>
-  </si>
-  <si>
-    <t>Mbeve Regina dos Santos talao 11566942</t>
-  </si>
-  <si>
-    <t>Muchanga Salvador Baptista bi 110202091364N</t>
-  </si>
-  <si>
-    <t>Muiambo Atalia Michaque c_eleit 1834033</t>
-  </si>
-  <si>
-    <t>Nhacale Aurora Dinis c_eleit 1550804</t>
-  </si>
-  <si>
-    <t>Roma Higino Francisco Carlos bi 110202136654P</t>
-  </si>
-  <si>
-    <t>Sitoe Avelina Azarias Sitoe c_nasc Xxxxxxxx</t>
-  </si>
-  <si>
-    <t>Sitoe Avelina Azarias Sitoe c_nasc xxxxxxxxx</t>
-  </si>
-  <si>
-    <t>Timana Fernando Manuel bi 3706723</t>
-  </si>
-  <si>
-    <t>Timbe Hercílio Timbe ced 45472</t>
-  </si>
-  <si>
-    <t>Tiua Regina Pedro bi 100402879917B</t>
-  </si>
-  <si>
-    <t>Uelane Saugina João c_eleit 2609439</t>
-  </si>
-  <si>
-    <t>Xerinda Filomena Marta bi 100390103W</t>
-  </si>
-  <si>
-    <t>Xerinda Julieta Augusto ced 69202</t>
-  </si>
-  <si>
-    <t>Xerinda Lizete Aurelio bi 110104918215I</t>
-  </si>
-  <si>
-    <t>Zimia Salmina Francisco bi 100405126306P</t>
-  </si>
-  <si>
-    <t>Zunguene Alberto c_eleit Xxxxx"</t>
+    <t>Admiro Vicente Massingue bi 100402879475P</t>
+  </si>
+  <si>
+    <t>Agostinho João Livisse bi 110104642611N</t>
+  </si>
+  <si>
+    <t>Albertina Kei Komaio c_eleit 12071563</t>
+  </si>
+  <si>
+    <t>Alberto Júlio Manganhe c_eleit 4807456</t>
+  </si>
+  <si>
+    <t>Alberto Magare Dava bi 100402255471S</t>
+  </si>
+  <si>
+    <t>Alberto Zunguene c_eleit Xxxxx</t>
+  </si>
+  <si>
+    <t>Alexandre Manuensa Melembe bi 100301713467C</t>
+  </si>
+  <si>
+    <t>Amélia Nhantsumbo bi 110202873403B</t>
+  </si>
+  <si>
+    <t>Ana Maria Antónia Mbeve bi 100005272F</t>
+  </si>
+  <si>
+    <t>Angela Carlos Xavier c_eleit 13747607</t>
+  </si>
+  <si>
+    <t>Angelina Iotassana Balate c_eleit 1004A580840212</t>
+  </si>
+  <si>
+    <t>Angelo Luis Macamo c_eleit 12071794</t>
+  </si>
+  <si>
+    <t>Antonio Mavulu Melembe Melembe bi 100098977X</t>
+  </si>
+  <si>
+    <t>Antonio muvulo Melembe bi 100098977x</t>
+  </si>
+  <si>
+    <t>Argentina Fernando Machai bi 110100290981F</t>
+  </si>
+  <si>
+    <t>Ariel Quingue Nhacolo bi 100402813194J</t>
+  </si>
+  <si>
+    <t>Arlindo Francisco Matsinhe talao 6654220</t>
+  </si>
+  <si>
+    <t>Artimiza Armando Chombela bi 110502813139I</t>
+  </si>
+  <si>
+    <t>Atalia Michaque Muiambo c_eleit 1834033</t>
+  </si>
+  <si>
+    <t>Aurora Dinis Nhacale c_eleit 1550804</t>
+  </si>
+  <si>
+    <t>Avelina Azarias Sitoe Sitoe c_nasc Xxxxxxxx</t>
+  </si>
+  <si>
+    <t>Avelina Azarias Sitoe Sitoe c_nasc xxxxxxxxx</t>
+  </si>
+  <si>
+    <t>Benedito Arlindo Chauque bi 110104370009B</t>
+  </si>
+  <si>
+    <t>Benedito Dinis Machaieie ced 65146</t>
+  </si>
+  <si>
+    <t>Benedito Diniz Machaeie ced 65146</t>
+  </si>
+  <si>
+    <t>Cacilda Armando Dimande c_eleit 576863</t>
+  </si>
+  <si>
+    <t>Carla Isabel Machiana p_port 15AJ41963</t>
+  </si>
+  <si>
+    <t>Carolina Alberto Nambal c_eleit 13454787</t>
+  </si>
+  <si>
+    <t>Cecília Rodrigues Cossa bi 100405892495N</t>
+  </si>
+  <si>
+    <t>Celeste Alfredo Homo bi 100405422384P</t>
+  </si>
+  <si>
+    <t>Celeste Gabriel Novela Chivure bi 110201649569Q</t>
+  </si>
+  <si>
+    <t>David Fernando Machaieie bi 100405710268N</t>
+  </si>
+  <si>
+    <t>Eduardo Alberto Zimia bi 100406013023F</t>
+  </si>
+  <si>
+    <t>Efigencia Alberto Mavundza bi 110102047742A</t>
+  </si>
+  <si>
+    <t>Elias Machelagodine Lumbela bi 110100295545A</t>
+  </si>
+  <si>
+    <t>Elias Raul Seth Langa bi 110200628536B</t>
+  </si>
+  <si>
+    <t>Erasmo Alberto Chambale Chambale bi 100406029175B</t>
+  </si>
+  <si>
+    <t>Ernesto Fernando Melembe ced 187227</t>
+  </si>
+  <si>
+    <t>Eugénio Alberto Chavana ced 46078</t>
+  </si>
+  <si>
+    <t>Ezequiel fenias Chiconela c_impost 5610</t>
+  </si>
+  <si>
+    <t>Fernando Ernesto Mulhanga bi 09020524751D</t>
+  </si>
+  <si>
+    <t>Fernando Manuel Timana bi 3706723</t>
+  </si>
+  <si>
+    <t>Fernando Paulino Xirinda c_cond 10731522</t>
+  </si>
+  <si>
+    <t>Filomena Cossa bi 2868605</t>
+  </si>
+  <si>
+    <t>Filomena Marta Xerinda bi 100390103W</t>
+  </si>
+  <si>
+    <t>Flora Silvestre Macuacua c_eleit 1004A860810839</t>
+  </si>
+  <si>
+    <t>Francisco Mucoi Pelembe bi 110100298852N</t>
+  </si>
+  <si>
+    <t>Franice Ernesto Mimbire bi 100401094341S</t>
+  </si>
+  <si>
+    <t>Gilda Alfredo Cossa bi 3293818</t>
+  </si>
+  <si>
+    <t>Hercílio Timbe Timbe ced 45472</t>
+  </si>
+  <si>
+    <t>Hermínio Ruben Mathombe bi 100406382003P</t>
+  </si>
+  <si>
+    <t>Higino Francisco Carlos Roma bi 110202136654P</t>
+  </si>
+  <si>
+    <t>Horácio Alberto Chauque bi 100404784848C</t>
+  </si>
+  <si>
+    <t>Idalina Macucule bi 100402553340I</t>
+  </si>
+  <si>
+    <t>Isabel Joaquim MANHIÇA bi 10006696B</t>
+  </si>
+  <si>
+    <t>Isaque Fenias Chiconela Chiconela c_impost 5610</t>
+  </si>
+  <si>
+    <t>Ismael Alfredo Chicuamba bi 100404696751Q</t>
+  </si>
+  <si>
+    <t>Januário Sozinho Sitoe ced 34170</t>
+  </si>
+  <si>
+    <t>Joana Afonso Cuna bi 100402079747F</t>
+  </si>
+  <si>
+    <t>José Diniz Machaeie ced 857421</t>
+  </si>
+  <si>
+    <t>José Paulo Timana Timana bi 110200350149S</t>
+  </si>
+  <si>
+    <t>Julieta Augusto Xerinda ced 69202</t>
+  </si>
+  <si>
+    <t>Laque Feliciano Timana bi 100405660468M</t>
+  </si>
+  <si>
+    <t>Latia fabiao Tivane bi 100405376506A</t>
+  </si>
+  <si>
+    <t>LAURINDA JOAQUIM MANHIÇA c_eleit 367707</t>
+  </si>
+  <si>
+    <t>Leonardo Fabião Mawelele c_eleit 12598423</t>
+  </si>
+  <si>
+    <t>Lizete Aurelio Xerinda bi 110104918215I</t>
+  </si>
+  <si>
+    <t>Lopes Alberto Zimia talao 6866173</t>
+  </si>
+  <si>
+    <t>Lopes Manuessa Melembe bi 1100101510857</t>
+  </si>
+  <si>
+    <t>Lúcia Clarmina Mapanga bi 100400667510Q</t>
+  </si>
+  <si>
+    <t>Luís Filipe Timana bi 100405892378M</t>
+  </si>
+  <si>
+    <t>Manuel Feniasse Matsinhe bi 110105100629A</t>
+  </si>
+  <si>
+    <t>Maria Azarias Chilaule bi 1004026800497N</t>
+  </si>
+  <si>
+    <t>Maria Azarias Chilaule ced 668046</t>
+  </si>
+  <si>
+    <t>Maria Azarias Chilaule Machaieie bi 100402680497N</t>
+  </si>
+  <si>
+    <t>Maria João Dolhana bi 100404559519P</t>
+  </si>
+  <si>
+    <t>Marta Alexandre Nhabinde Mbebe bi 110100338532J</t>
+  </si>
+  <si>
+    <t>Marta Causolada Macuacua c_eleit 13082829</t>
+  </si>
+  <si>
+    <t>Mónica Amone Massango bi 110101302568F</t>
+  </si>
+  <si>
+    <t>Moseis Antonio Matosse bi 100402005836B</t>
+  </si>
+  <si>
+    <t>Regina dos Santos Mbeve talao 11566942</t>
+  </si>
+  <si>
+    <t>Regina Pedro Tiua bi 100402879917B</t>
+  </si>
+  <si>
+    <t>Salmina Francisco Zimia bi 100405126306P</t>
+  </si>
+  <si>
+    <t>Salvador Baptista Muchanga bi 110202091364N</t>
+  </si>
+  <si>
+    <t>Saugina João Uelane c_eleit 2609439</t>
+  </si>
+  <si>
+    <t>Sebastião Lopes Timane bi 100402813277B</t>
+  </si>
+  <si>
+    <t>Sérgio Augusto Massingue Massingue bi 100401395656S</t>
+  </si>
+  <si>
+    <t>Sérgio Gonçalves Hunguana bi 110101036908C</t>
+  </si>
+  <si>
+    <t>Talita Alfredo Ricotso bi 100401094250B</t>
+  </si>
+  <si>
+    <t>Violeta Cotassana MANHIÇA bi 100400613064B</t>
   </si>
 </sst>
 </file>
@@ -796,7 +940,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -869,12 +1013,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1455,35 +1593,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.25" style="11" customWidth="1"/>
-    <col min="2" max="2" width="20.25" style="16" customWidth="1"/>
-    <col min="3" max="3" width="61.625" style="11" customWidth="1"/>
+    <col min="1" max="1" width="29.19921875" style="11" customWidth="1"/>
+    <col min="2" max="2" width="20.19921875" style="16" customWidth="1"/>
+    <col min="3" max="3" width="61.59765625" style="11" customWidth="1"/>
     <col min="4" max="4" width="27" style="11" customWidth="1"/>
-    <col min="5" max="5" width="14.125" style="11" customWidth="1"/>
-    <col min="6" max="6" width="46.625" style="11" customWidth="1"/>
-    <col min="7" max="7" width="19.875" style="11" customWidth="1"/>
-    <col min="8" max="8" width="8.625" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.375" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.625" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.09765625" style="11" customWidth="1"/>
+    <col min="6" max="6" width="46.59765625" style="11" customWidth="1"/>
+    <col min="7" max="7" width="19.8984375" style="11" customWidth="1"/>
+    <col min="8" max="8" width="8.59765625" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.3984375" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.59765625" style="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="69.125" style="11" customWidth="1"/>
+    <col min="12" max="12" width="69.09765625" style="11" customWidth="1"/>
     <col min="13" max="13" width="47.5" style="11" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.125" style="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.25" style="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.09765625" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.19921875" style="11" bestFit="1" customWidth="1"/>
     <col min="17" max="16384" width="11" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="13" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="13" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1533,7 +1671,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>16</v>
       </c>
@@ -1541,7 +1679,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="23" t="s">
         <v>31</v>
       </c>
@@ -1552,19 +1690,19 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" s="25" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
         <v>26</v>
       </c>
       <c r="B4" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="34" t="s">
         <v>84</v>
       </c>
       <c r="I4" s="23"/>
     </row>
-    <row r="5" spans="1:16" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
         <v>28</v>
       </c>
@@ -1581,7 +1719,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" s="25" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="23" t="s">
         <v>17</v>
       </c>
@@ -1598,7 +1736,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="30" t="s">
         <v>23</v>
       </c>
@@ -1618,7 +1756,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="30" t="s">
         <v>23</v>
       </c>
@@ -1641,7 +1779,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:16" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="30" t="s">
         <v>33</v>
       </c>
@@ -1655,7 +1793,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>36</v>
       </c>
@@ -1669,7 +1807,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="19" t="s">
         <v>36</v>
       </c>
@@ -1683,7 +1821,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>37</v>
       </c>
@@ -1699,25 +1837,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D67"/>
+  <dimension ref="A1:D119"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D58" sqref="D58"/>
+      <selection pane="bottomRight" activeCell="A67" sqref="A67:A119"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="26.625" style="10" customWidth="1"/>
+    <col min="1" max="1" width="12.3984375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="26.59765625" style="10" customWidth="1"/>
     <col min="3" max="3" width="41.5" style="4" customWidth="1"/>
-    <col min="4" max="4" width="41.625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.875" style="4"/>
+    <col min="4" max="4" width="41.59765625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.8984375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
@@ -1731,12 +1869,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="9"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
         <v>18</v>
       </c>
@@ -1747,7 +1885,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="27" t="s">
         <v>18</v>
       </c>
@@ -1758,7 +1896,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="27" t="s">
         <v>18</v>
       </c>
@@ -1769,7 +1907,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="27" t="s">
         <v>18</v>
       </c>
@@ -1780,7 +1918,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
         <v>18</v>
       </c>
@@ -1791,7 +1929,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="27" t="s">
         <v>18</v>
       </c>
@@ -1802,7 +1940,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="27" t="s">
         <v>18</v>
       </c>
@@ -1813,7 +1951,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="27" t="s">
         <v>18</v>
       </c>
@@ -1824,7 +1962,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="27" t="s">
         <v>18</v>
       </c>
@@ -1835,7 +1973,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="27" t="s">
         <v>18</v>
       </c>
@@ -1846,7 +1984,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="27" t="s">
         <v>18</v>
       </c>
@@ -1857,7 +1995,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="27" t="s">
         <v>18</v>
       </c>
@@ -1868,7 +2006,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="27" t="s">
         <v>18</v>
       </c>
@@ -1879,568 +2017,1140 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" s="17"/>
     </row>
-    <row r="17" spans="1:3" s="33" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="34">
+      <c r="B17">
+        <v>4502</v>
+      </c>
+      <c r="C17" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" s="33" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18">
+        <v>9815</v>
+      </c>
+      <c r="C18" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19">
+        <v>9580</v>
+      </c>
+      <c r="C19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20">
+        <v>4436</v>
+      </c>
+      <c r="C20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21">
+        <v>4398</v>
+      </c>
+      <c r="C21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22">
+        <v>9103</v>
+      </c>
+      <c r="C22" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23">
+        <v>4003</v>
+      </c>
+      <c r="C23" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24">
+        <v>4515</v>
+      </c>
+      <c r="C24" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25">
+        <v>9732</v>
+      </c>
+      <c r="C25" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26">
+        <v>9247</v>
+      </c>
+      <c r="C26" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27">
+        <v>4947</v>
+      </c>
+      <c r="C27" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28">
+        <v>4897</v>
+      </c>
+      <c r="C28" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29">
+        <v>9695</v>
+      </c>
+      <c r="C29" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30">
+        <v>4002</v>
+      </c>
+      <c r="C30" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31">
+        <v>4004</v>
+      </c>
+      <c r="C31" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32">
+        <v>4170</v>
+      </c>
+      <c r="C32" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>4758</v>
+      </c>
+      <c r="C33" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>4407</v>
+      </c>
+      <c r="C34" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35">
+        <v>4927</v>
+      </c>
+      <c r="C35" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36">
+        <v>9511</v>
+      </c>
+      <c r="C36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37">
+        <v>9704</v>
+      </c>
+      <c r="C37" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38">
+        <v>9006</v>
+      </c>
+      <c r="C38" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B39">
+        <v>9896</v>
+      </c>
+      <c r="C39" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B40">
+        <v>4802</v>
+      </c>
+      <c r="C40" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A41" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B41">
+        <v>9209</v>
+      </c>
+      <c r="C41" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A42" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B42">
+        <v>9756</v>
+      </c>
+      <c r="C42" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A43" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B43">
+        <v>9759</v>
+      </c>
+      <c r="C43" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A44" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B44">
+        <v>9766</v>
+      </c>
+      <c r="C44" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A45" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B45">
+        <v>9786</v>
+      </c>
+      <c r="C45" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A46" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B46">
+        <v>9303</v>
+      </c>
+      <c r="C46" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A47" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B47">
+        <v>9311</v>
+      </c>
+      <c r="C47" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A48" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B48">
+        <v>9282</v>
+      </c>
+      <c r="C48" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A49" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B49">
+        <v>9733</v>
+      </c>
+      <c r="C49" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A50" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B50">
+        <v>4903</v>
+      </c>
+      <c r="C50" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A51" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B51">
+        <v>4862</v>
+      </c>
+      <c r="C51" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A52" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B52">
+        <v>9746</v>
+      </c>
+      <c r="C52" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A53" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B53">
+        <v>9236</v>
+      </c>
+      <c r="C53" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A54" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B54">
+        <v>4363</v>
+      </c>
+      <c r="C54" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A55" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B55">
+        <v>4419</v>
+      </c>
+      <c r="C55" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A56" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B56">
+        <v>4753</v>
+      </c>
+      <c r="C56" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A57" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B57">
+        <v>9223</v>
+      </c>
+      <c r="C57" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A58" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B58">
+        <v>9229</v>
+      </c>
+      <c r="C58" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A59" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B59">
+        <v>8436</v>
+      </c>
+      <c r="C59" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A60" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B60">
+        <v>4543</v>
+      </c>
+      <c r="C60" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A61" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B61">
+        <v>4763</v>
+      </c>
+      <c r="C61" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A62" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B62">
         <v>9989</v>
       </c>
-      <c r="C17" s="33" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="35">
+      <c r="C62" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A63" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B63">
+        <v>4583</v>
+      </c>
+      <c r="C63" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A64" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B64">
+        <v>9585</v>
+      </c>
+      <c r="C64" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A65" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B65">
+        <v>4755</v>
+      </c>
+      <c r="C65" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A66" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B66">
+        <v>9198</v>
+      </c>
+      <c r="C66" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A67" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B67">
+        <v>9273</v>
+      </c>
+      <c r="C67" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A68" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B68">
+        <v>9744</v>
+      </c>
+      <c r="C68" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A69" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B69">
+        <v>9284</v>
+      </c>
+      <c r="C69" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A70" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B70">
+        <v>4554</v>
+      </c>
+      <c r="C70" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A71" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B71">
+        <v>4362</v>
+      </c>
+      <c r="C71" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A72" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B72">
+        <v>9853</v>
+      </c>
+      <c r="C72" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A73" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B73">
+        <v>4229</v>
+      </c>
+      <c r="C73" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A74" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B74">
+        <v>9225</v>
+      </c>
+      <c r="C74" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A75" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B75">
+        <v>4314</v>
+      </c>
+      <c r="C75" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A76" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B76">
+        <v>9749</v>
+      </c>
+      <c r="C76" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A77" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B77">
+        <v>9234</v>
+      </c>
+      <c r="C77" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A78" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B78">
         <v>9940</v>
       </c>
-      <c r="C18" s="33" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="17">
+      <c r="C78" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A79" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B79">
         <v>9745</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" s="17">
+      <c r="C79" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A80" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B80">
+        <v>9028</v>
+      </c>
+      <c r="C80" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A81" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B81">
+        <v>9029</v>
+      </c>
+      <c r="C81" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A82" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B82">
+        <v>9032</v>
+      </c>
+      <c r="C82" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A83" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B83">
+        <v>9082</v>
+      </c>
+      <c r="C83" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A84" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B84">
+        <v>4754</v>
+      </c>
+      <c r="C84" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A85" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B85">
+        <v>9311</v>
+      </c>
+      <c r="C85" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A86" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B86">
+        <v>4356</v>
+      </c>
+      <c r="C86" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A87" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B87">
+        <v>9770</v>
+      </c>
+      <c r="C87" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A88" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B88">
+        <v>4913</v>
+      </c>
+      <c r="C88" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A89" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B89">
+        <v>4233</v>
+      </c>
+      <c r="C89" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A90" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B90">
+        <v>9235</v>
+      </c>
+      <c r="C90" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A91" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B91">
+        <v>9691</v>
+      </c>
+      <c r="C91" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A92" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B92">
+        <v>9327</v>
+      </c>
+      <c r="C92" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A93" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B93">
+        <v>4420</v>
+      </c>
+      <c r="C93" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A94" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B94">
+        <v>4001</v>
+      </c>
+      <c r="C94" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A95" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B95">
+        <v>9720</v>
+      </c>
+      <c r="C95" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A96" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B96">
+        <v>4378</v>
+      </c>
+      <c r="C96" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A97" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B97">
+        <v>4406</v>
+      </c>
+      <c r="C97" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A98" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B98">
         <v>9209</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="17">
-        <v>9310</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B22" s="17">
+      <c r="C98" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A99" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B99">
+        <v>9303</v>
+      </c>
+      <c r="C99" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A100" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B100">
         <v>9311</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B23" s="17">
+      <c r="C100" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A101" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B101">
         <v>9756</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B24" s="17">
+      <c r="C101" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A102" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B102">
         <v>9759</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B25" s="17">
+      <c r="C102" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A103" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B103">
         <v>9766</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B26" s="17">
-        <v>9236</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B27" s="17">
+      <c r="C103" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A104" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B104">
+        <v>9786</v>
+      </c>
+      <c r="C104" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A105" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B105">
         <v>9580</v>
       </c>
-      <c r="C27" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B28" s="17">
+      <c r="C105" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A106" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B106">
+        <v>9748</v>
+      </c>
+      <c r="C106" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A107" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B107">
+        <v>9265</v>
+      </c>
+      <c r="C107" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A108" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B108">
+        <v>9735</v>
+      </c>
+      <c r="C108" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A109" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B109">
+        <v>4007</v>
+      </c>
+      <c r="C109" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A110" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B110">
+        <v>9712</v>
+      </c>
+      <c r="C110" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A111" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B111">
+        <v>9722</v>
+      </c>
+      <c r="C111" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A112" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B112">
+        <v>9703</v>
+      </c>
+      <c r="C112" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A113" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B113">
+        <v>9686</v>
+      </c>
+      <c r="C113" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A114" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B114">
+        <v>9263</v>
+      </c>
+      <c r="C114" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A115" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B115">
+        <v>4313</v>
+      </c>
+      <c r="C115" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A116" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B116">
+        <v>4815</v>
+      </c>
+      <c r="C116" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A117" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B117">
         <v>9231</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B29" s="17">
-        <v>9876</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B30" s="17">
-        <v>9815</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B31" s="17">
-        <v>9223</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32" s="17">
-        <v>9695</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B33" s="17">
-        <v>9310</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B34" s="17">
-        <v>9311</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B35" s="17">
-        <v>9311</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B36" s="17">
-        <v>9756</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B37" s="17">
-        <v>9759</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B38" s="17">
-        <v>9766</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B39" s="17">
-        <v>9786</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B40" s="17">
-        <v>9209</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B41" s="17">
-        <v>9786</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B42" s="17">
-        <v>9733</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B43" s="17">
-        <v>9744</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B44" s="17">
-        <v>9265</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B45" s="17">
-        <v>9234</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B46" s="17">
-        <v>9235</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B47" s="17">
+      <c r="C117" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A118" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B118">
+        <v>4559</v>
+      </c>
+      <c r="C118" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A119" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B119">
         <v>9741</v>
       </c>
-      <c r="C47" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B48" s="17">
-        <v>9720</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B49" s="17">
-        <v>9735</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B50" s="17">
-        <v>9691</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B51" s="17">
-        <v>9247</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B52" s="17">
-        <v>9712</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B53" s="17">
-        <v>9686</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B54" s="17">
-        <v>9511</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B55" s="17">
-        <v>9704</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B56" s="17">
-        <v>9225</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B57" s="17">
-        <v>9006</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B58" s="17">
-        <v>9896</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B59" s="17">
-        <v>9585</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B60" s="17">
-        <v>9853</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B61" s="17">
-        <v>9722</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B62" s="17">
-        <v>9263</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B63" s="17">
-        <v>9273</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B64" s="17">
-        <v>9770</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B65" s="17">
-        <v>9327</v>
-      </c>
-      <c r="C65" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B66" s="17">
-        <v>9703</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B67" s="17">
-        <v>9104</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>126</v>
+      <c r="C119" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -2454,20 +3164,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="24.875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="15.875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="49.875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="29.09765625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="24.8984375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="15.8984375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="49.8984375" style="3" customWidth="1"/>
     <col min="5" max="16384" width="11" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>19</v>
       </c>
@@ -2481,7 +3191,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>74</v>
       </c>
@@ -2489,7 +3199,7 @@
         <v>75</v>
       </c>
       <c r="C2" s="5">
-        <v>201710181</v>
+        <v>201802011</v>
       </c>
       <c r="D2" s="30" t="s">
         <v>83</v>

</xml_diff>